<commit_message>
ccdi  - all 5 tabs added (total - 2 scripts)
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation0919\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\CCDI scripts\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E6DB14-414A-4D12-BC62-A0DD45893927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D949CBB1-4783-4B63-BA01-7F8328975025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>WebExcel</t>
   </si>
@@ -56,25 +56,6 @@
   </si>
   <si>
     <t>ParticipantsTab</t>
-  </si>
-  <si>
-    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-WHERE st.phs_accession IN ['phs003111']
-        OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-        OPTIONAL MATCH (p)-[:of_clinical_measure_file_participant]-(cmfp:clinical_measure_file)
-        OPTIONAL MATCH (st)&lt;-[:of_clinical_measure_file]-(cmf:clinical_measure_file)
-        OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(rf:radiology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_pathology_file]-(pf:pathology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_methylation_array_file]-(maf:methylation_array_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_single_cell_sequencing_file]-(scsf:single_cell_sequencing_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_sequencing_file]-(sf:sequencing_file)
-        WITH cmfp, cmf, rf, pf, maf, scsf, sf, p, st, sm, dg
-        return
-        count(distinct st.id) as Studies,
-        count(distinct p.id)as Participants,
-        count(distinct sm.id) as Samples,
-        count(distinct cmfp.id) + count(distinct cmf.id) + count(distinct rf.id) + count(distinct pf.id) + count(distinct maf.id) + count(distinct scsf.id) + count(distinct sf.id) as Files</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;--(p:participant)&lt;--(dia:diagnosis)
@@ -88,6 +69,289 @@
 coalesce(p.ethnicity, '') AS `Ethnicity` ,
 coalesce(p.alternate_participant_id, '') AS `Alternate ID`
 Order by p.participant_id Limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[:of_participant]-(p:participant)
+WHERE s.phs_accession IN ['phs003111']
+        OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+        OPTIONAL MATCH (p)-[:of_clinical_measure_file_participant]-(cmfp:clinical_measure_file)
+        OPTIONAL MATCH (s)&lt;-[:of_clinical_measure_file]-(cmf:clinical_measure_file)
+        OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(rf:radiology_file)
+        OPTIONAL MATCH (sm)&lt;-[:of_pathology_file]-(pf:pathology_file)
+        OPTIONAL MATCH (sm)&lt;-[:of_methylation_array_file]-(maf:methylation_array_file)
+        OPTIONAL MATCH (sm)&lt;-[:of_single_cell_sequencing_file]-(scsf:single_cell_sequencing_file)
+        OPTIONAL MATCH (sm)&lt;-[:of_sequencing_file]-(sf:sequencing_file)
+        WITH cmfp, cmf, rf, pf, maf, scsf, sf, p, s, sm, dg
+        return
+        count(distinct s.id) as Studies,
+        count(distinct p.id)as Participants,
+        count(distinct sm.id) as Samples,
+        count(distinct cmfp.id) + count(distinct cmf.id) + count(distinct rf.id) + count(distinct pf.id) + count(distinct maf.id) + count(distinct scsf.id) + count(distinct sf.id) as Files</t>
+  </si>
+  <si>
+    <t>DiagnosisTab</t>
+  </si>
+  <si>
+    <t>StudiesTab</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
+where s.phs_accession = "phs003111"
+OPTIONAL MATCH(fo:follow_up)--&gt;(p)
+with distinct d, p, s, fo
+return
+coalesce(p.participant_id, '') as `Participant ID`,
+coalesce(s.phs_accession, '') as `Study Accession`,
+coalesce(d.diagnosis_icd_o, '') as `ICD-O Morphology`,
+coalesce(d.disease_phase, '') as `Disease Phase`,
+coalesce(d.anatomic_site, '') as `Anatomic Site`,
+coalesce(d.age_at_diagnosis, '') as `Age at diagnosis (days)`,
+coalesce(fo.vital_status, '') as `Vital Status`
+Order by p.participant_id Limit 100</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (p:participant)&lt;-[:of_sample]-(sm:sample)
+        MATCH (s:study)&lt;-[:of_participant]-(p)
+WHERE s.phs_accession IN ['phs003111']
+        WITH p, s, sm
+        RETURN DISTINCT
+          sm.sample_id as `Sample ID`,
+          p.participant_id as `Participant ID`,
+          s.study_id as `Study ID`,
+          sm.anatomic_site as `Anatomic Site`,
+          sm.participant_age_at_collection as `Age at Sample Collection`,
+          sm.diagnosis_icd_o as `Sample ICD-O Morphology`,
+          sm.sample_tumor_status as `Sample Tumor Status`,
+          sm.tumor_classification as `Sample Tumor Classification`
+Order by sm.sample_id Limit 100
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (file:clinical_measure_file)
+MATCH (p:participant)-[:of_clinical_measure_file_participant]-(file)
+MATCH (st)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p, ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units, toInteger(floor(log(file.file_size)/log(1024))) as i, 2 as precision
+WITH file, st, p,
+file.file_size /(1024^i) AS value, 10^precision AS factor, units[i] as unit
+WITH file, st, p, unit, round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Clinical measure' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+null AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:clinical_measure_file)
+MATCH (st:study)&lt;-[:of_clinical_measure_file]-(file)
+where st.phs_accession in ['phs003111']
+WITH file, st,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Clinical measure' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+null as `Participant ID`,
+null AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:methylation_array_file)
+MATCH (sm:sample)&lt;-[:of_methylation_array_file]-(file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm)
+MATCH (st:study)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p, sm,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st, p, sm,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, p, sm, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Methylation array' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+sm.sample_id AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:pathology_file)
+MATCH (sm:sample)&lt;-[:of_pathology_file]-(file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm)
+MATCH (st:study)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p, sm,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st, p, sm,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, p, sm, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Pathology imaging' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+sm.sample_id AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:radiology_file)
+MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
+MATCH (st:study)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st, p,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, p, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Radiology imaging' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+null AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:single_cell_sequencing_file)
+MATCH (sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm)
+MATCH (st:study)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p, sm,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st, p, sm,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, p, sm, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Single Cell Sequencing' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+sm.sample_id AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+UNION ALL
+MATCH (file:sequencing_file)
+MATCH (sm:sample)&lt;-[:of_sequencing_file]-(file)
+MATCH (p:participant)&lt;-[:of_sample]-(sm)
+MATCH (st:study)&lt;-[:of_participant]-(p)
+where st.phs_accession in ['phs003111']
+WITH file, st, p, sm,
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(file.file_size)/log(1024))) as i,
+2 as precision
+WITH file, st, p, sm,
+file.file_size /(1024^i) AS value,
+10^precision AS factor,
+units[i] as unit
+WITH file, st, p, sm, unit,
+round(factor * value)/factor AS size
+RETURN DISTINCT
+file.file_name AS `File Name`,
+'Sequencing' AS `File Category`,
+file.file_description AS `File Description`,
+file.file_type AS `File Type`,
+CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
+st.study_id AS `Study ID`,
+p.participant_id as `Participant ID`,
+sm.sample_id AS `Sample ID`,
+file.dcf_indexd_guid AS `GUID`,
+file.md5sum AS `MD5sum`
+ </t>
+  </si>
+  <si>
+    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+where st.phs_accession in ["phs003111"]
+  with st, count(p) as num_p
+        MATCH (st:study)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+        with st, num_p, dg.diagnosis_icd_o as dg_cancers, count(dg.diagnosis_icd_o) as num_cancers
+        ORDER BY num_cancers desc
+        with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
+        MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
+        with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
+        ORDER BY num_sites desc
+        with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
+        MATCH (st)&lt;-[*..3]-(fl)        WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:rathology OR fl:methylation_array_file OR fl:single_cell_sequencing_file)
+        with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
+        ORDER BY num_ft desc
+        with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
+        MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm:sample)
+        WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm.sample_id) as num_samples
+        MATCH (st)&lt;-[*..3]-(file)
+ WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:rathology OR file:methylation_array_file OR file:single_cell_sequencing_file)
+        OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+        OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+        WHERE stp.personnel_type = 'PI'
+        OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+        WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
+        order by st.study_id
+        RETURN DISTINCT
+          st.study_short_title as `Study Short Title`,
+        st.study_id as `Study ID`,
+          CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "..."  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
+         CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "..."  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
+         num_p as `Number of Participants`,
+          num_samples as `Number of Samples`,
+          num_files as `Number of Files`,
+         CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "..."  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
+         apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
+         apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
+         apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
 </sst>
 </file>
@@ -459,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,15 +753,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -506,21 +770,73 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+    <row r="5" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
CCDI - corrected 2 base scripts with the updated queries from Wei.
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\OctBranch\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FD5850-4EEB-4365-B7FC-25A25AB16340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FD3AD9-768E-4974-A2FB-4E93F0DB4293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -58,25 +58,6 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[:of_participant]-(p:participant)
-WHERE s.phs_accession IN ['phs003111']
-        OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-        OPTIONAL MATCH (p)-[:of_clinical_measure_file_participant]-(cmfp:clinical_measure_file)
-        OPTIONAL MATCH (s)&lt;-[:of_clinical_measure_file]-(cmf:clinical_measure_file)
-        OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(rf:radiology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_pathology_file]-(pf:pathology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_methylation_array_file]-(maf:methylation_array_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_single_cell_sequencing_file]-(scsf:single_cell_sequencing_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_sequencing_file]-(sf:sequencing_file)
-        WITH cmfp, cmf, rf, pf, maf, scsf, sf, p, s, sm, dg
-        return
-        count(distinct s.id) as Studies,
-        count(distinct p.id)as Participants,
-        count(distinct sm.id) as Samples,
-        count(distinct cmfp.id) + count(distinct cmf.id) + count(distinct rf.id) + count(distinct pf.id) + count(distinct maf.id) + count(distinct scsf.id) + count(distinct sf.id) as Files</t>
-  </si>
-  <si>
     <t>DiagnosisTab</t>
   </si>
   <si>
@@ -89,276 +70,386 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (p:participant)&lt;-[:of_sample]-(sm:sample)
-        MATCH (s:study)&lt;-[:of_participant]-(p)
-WHERE s.phs_accession IN ['phs003111']
-        WITH p, s, sm
-        RETURN DISTINCT
-          sm.sample_id as `Sample ID`,
-          p.participant_id as `Participant ID`,
-          s.study_id as `Study ID`,
-          sm.anatomic_site as `Anatomic Site`,
-          sm.participant_age_at_collection as `Age at Sample Collection`,
-          sm.diagnosis_icd_o as `Sample ICD-O Morphology`,
-          sm.sample_tumor_status as `Sample Tumor Status`,
-          sm.tumor_classification as `Sample Tumor Classification`
-Order by sm.sample_id Limit 100
-          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (file:clinical_measure_file)
-MATCH (p:participant)-[:of_clinical_measure_file_participant]-(file)
-MATCH (st)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p, ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units, toInteger(floor(log(file.file_size)/log(1024))) as i, 2 as precision
-WITH file, st, p,
-file.file_size /(1024^i) AS value, 10^precision AS factor, units[i] as unit
-WITH file, st, p, unit, round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Clinical measure' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-null AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:clinical_measure_file)
-MATCH (st:study)&lt;-[:of_clinical_measure_file]-(file)
-where st.phs_accession in ['phs003111']
-WITH file, st,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Clinical measure' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-null as `Participant ID`,
-null AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:methylation_array_file)
-MATCH (sm:sample)&lt;-[:of_methylation_array_file]-(file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm)
-MATCH (st:study)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p, sm,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st, p, sm,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, p, sm, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Methylation array' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-sm.sample_id AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:pathology_file)
-MATCH (sm:sample)&lt;-[:of_pathology_file]-(file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm)
-MATCH (st:study)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p, sm,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st, p, sm,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, p, sm, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Pathology imaging' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-sm.sample_id AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:radiology_file)
-MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
-MATCH (st:study)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st, p,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, p, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Radiology imaging' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-null AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:single_cell_sequencing_file)
-MATCH (sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm)
-MATCH (st:study)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p, sm,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st, p, sm,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, p, sm, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Single Cell Sequencing' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-sm.sample_id AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
-UNION ALL
-MATCH (file:sequencing_file)
-MATCH (sm:sample)&lt;-[:of_sequencing_file]-(file)
-MATCH (p:participant)&lt;-[:of_sample]-(sm)
-MATCH (st:study)&lt;-[:of_participant]-(p)
-where st.phs_accession in ['phs003111']
-WITH file, st, p, sm,
-['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-toInteger(floor(log(file.file_size)/log(1024))) as i,
-2 as precision
-WITH file, st, p, sm,
-file.file_size /(1024^i) AS value,
-10^precision AS factor,
-units[i] as unit
-WITH file, st, p, sm, unit,
-round(factor * value)/factor AS size
-RETURN DISTINCT
-file.file_name AS `File Name`,
-'Sequencing' AS `File Category`,
-file.file_description AS `File Description`,
-file.file_type AS `File Type`,
-CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
-st.study_id AS `Study ID`,
-p.participant_id as `Participant ID`,
-sm.sample_id AS `Sample ID`,
-file.dcf_indexd_guid AS `GUID`,
-file.md5sum AS `MD5sum`
- </t>
-  </si>
-  <si>
-    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-where st.phs_accession in ["phs003111"]
-  with st, count(p) as num_p
-        MATCH (st:study)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
-        with st, num_p, dg.diagnosis_icd_o as dg_cancers, count(dg.diagnosis_icd_o) as num_cancers
-        ORDER BY num_cancers desc
-        with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
-        MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
-        with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
-        ORDER BY num_sites desc
-        with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
-        MATCH (st)&lt;-[*..3]-(fl)        WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:rathology OR fl:methylation_array_file OR fl:single_cell_sequencing_file)
-        with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
-        ORDER BY num_ft desc
-        with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
-        MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm:sample)
-        WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm.sample_id) as num_samples
-        MATCH (st)&lt;-[*..3]-(file)
- WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:rathology OR file:methylation_array_file OR file:single_cell_sequencing_file)
-        OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-        OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-        WHERE stp.personnel_type = 'PI'
-        OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-        WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
-        order by st.study_id
-        RETURN DISTINCT
-          st.study_short_title as `Study Short Title`,
-        st.study_id as `Study ID`,
-          CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "..."  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
-         CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "..."  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
-         num_p as `Number of Participants`,
-          num_samples as `Number of Samples`,
-          num_files as `Number of Files`,
-         CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "..."  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
-         apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
-         apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
-         apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(dia:diagnosis)
+    <t>MATCH (s:study)&lt;--(p:participant)
 WHERE s.phs_accession IN ['phs003111']
 WITH DISTINCT p, s
 RETURN
 coalesce(p.participant_id, '') AS `Participant ID`,
 coalesce(s.phs_accession, '') AS `Study ID`,
-coalesce(p.gender, '') AS `Gender` ,
+coalesce(p.sex_at_birth, '') AS `Sex` ,
 coalesce(p.race, '') AS `Race`,
 coalesce(p.ethnicity, '') AS `Ethnicity` ,
 coalesce(p.alternate_participant_id, '') AS `Alternate ID`
 Order by p.participant_id Limit 100</t>
   </si>
   <si>
-    <t xml:space="preserve">Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
+    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+WHERE  st.phs_accession IN ['phs003111']
+        OPTIONAL MATCH (st)&lt;-[*..5]-(file)
+        WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:rathology OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+        WITH file, p, st, sm
+        return
+        count(distinct st.id) as Studies,
+        count(distinct p.id)as Participants,
+          count(distinct sm.id) as Samples,
+        count(distinct file.id) as Files</t>
+  </si>
+  <si>
+    <t>CALL {
+MATCH (file:clinical_measure_file)
+        MATCH (p:participant)-[:of_clinical_measure_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Clinical data' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        "" AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:clinical_measure_file)
+        MATCH (st:study)&lt;-[:of_clinical_measure_file]-(file)
+        Where st.phs_accession in ['phs003111']
+        with file, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Clinical data' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        "" as participant_id,
+        "" AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:methylation_array_file)
+        MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_methylation_array_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, sm1, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, sm1, sm, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, sm1, sm, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Methylation array' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+                    ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:pathology_file)
+        MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_pathology_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, sm1, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, sm1, sm, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, sm1, sm, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Pathology imaging' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+                    ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:radiology_file)
+        MATCH (p:participant)&lt;-[:of_radiology_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Radiology imaging' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        "" AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:single_cell_sequencing_file)
+        MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_single_cell_sequencing_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, sm1, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, sm1, sm, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, sm1, sm, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Single Cell Sequencing' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+                    ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:sequencing_file)
+        MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_sequencing_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, sm1, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, sm1, sm, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, sm1, sm, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Sequencing' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+                    ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file:cytogenomic_file)
+        MATCH (p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;-[*0..2]-(sm:sample)&lt;-[:of_cytogenomic_file]-(file)
+        MATCH (st:study)&lt;-[:of_participant]-(p)
+        Where st.phs_accession in ['phs003111']
+        with file, p, sm1, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, p, sm1, sm, st,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, p, sm1, sm, st, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        'Cytogenomic' AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        p.participant_id as participant_id,
+        CASE sm1.sample_id WHEN sm.sample_id THEN sm.sample_id
+                    ELSE sm1.sample_id + ',' + sm.sample_id END AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+        UNION ALL
+        MATCH (file)
+        WHERE (file:sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+        MATCH (st:study)&lt;-[:of_cell_line|of_pdx]-(cl)&lt;--(sm:sample)
+        Where (cl: cell_line or cl: pdx) and st.phs_accession in ['phs003111']
+        MATCH (sm)&lt;--(file)
+        with file, sm, st,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(file.file_size)/log(1024))) as i,
+        2 as precision
+        WITH file, st, sm,
+        file.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+        WITH file, st, sm, unit,
+        round(factor * value)/factor AS size
+        RETURN DISTINCT
+        file.file_name AS file_name,
+        CASE LABELS(file)[0]
+                WHEN 'sequencing_file' THEN 'Sequencing'
+                WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                WHEN 'pathology_file' THEN 'Pathology imaging'
+                WHEN 'methylation_array_file' THEN 'Methylation array' END AS file_category,
+        file.file_description AS file_description,
+        file.file_type AS file_type,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS file_size,
+        st.study_id AS study_id,
+        "" as participant_id,
+        sm.sample_id AS sample_id,
+        file.dcf_indexd_guid AS guid,
+        file.md5sum AS md5sum
+}
+RETURN file_name AS `File Name`,
+file_category As `File Category`,
+file_description As `File Description`,
+file_type As `File Type`,
+file_size As `File Size`,
+study_id As `Study ID`,
+participant_id As `Participant ID`,
+sample_id As `Sample ID`,
+guid As `GUID`,
+md5sum As `MD5Sum`
+ORDER BY file_name LIMIT 100</t>
+  </si>
+  <si>
+    <t>CALL {
+  MATCH (st:study)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm:sample)
+  WHERE (pcp:participant or pcp:cell_line or pcp:pdx) and st.phs_accession IN ['phs003111']
+  return st, case labels(pcp)[0] when "participant" then pcp.participant_id else "" end as participant_id, sm
+  union all
+  MATCH (st:study)&lt;-[:of_participant]-(p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
+  WHERE (cp:cell_line or cp:pdx) and st.phs_accession IN ['phs003111']
+  with st, p.participant_id as participant_id, [sm1,sm2] as sampleArr
+  unwind sampleArr as sm
+  return st, participant_id, sm
+}
+RETURN DISTINCT
+          sm.sample_id as `Sample ID`,
+          participant_id as `Participant ID`,
+          st.study_id as `Study ID`,
+          sm.anatomic_site as `Anatomic Site`,
+          case sm.participant_age_at_collection when -999 then 'Not Reported' else coalesce(sm.participant_age_at_collection, '') end as `Age at Sample Collection`,
+          coalesce(sm.diagnosis_classification, '') as `Diagnosis`,
+          coalesce(sm.diagnosis_classification_system, '') as `Diagnosis Classification System`,
+          coalesce(sm.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
+          coalesce(sm.diagnosis_basis, '') as `Diagnosis Basis`,
+          coalesce(sm.diagnosis_comment, '') as `Diagnosis Comment`,
+          sm.sample_tumor_status as `Sample Tumor Status`,
+          sm.tumor_classification as `Sample Tumor Classification`
+Order by sm.sample_id Limit 100</t>
+  </si>
+  <si>
+    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
 where s.phs_accession = "phs003111"
 OPTIONAL MATCH(fo:follow_up)--&gt;(p)
 with distinct d, p, s, fo
 return
 coalesce(p.participant_id, '') as `Participant ID`,
 coalesce(s.phs_accession, '') as `Study ID`,
-coalesce(d.diagnosis_icd_o, '') as `Diagnosis (ICD-O)`,
+coalesce(d.diagnosis_classification, '') as `Diagnosis`,
+coalesce(d.diagnosis_classification_system, '') as `Diagnosis Classification System`,
+coalesce(d.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
+coalesce(d.diagnosis_basis, '') as `Diagnosis Basis`,
+coalesce(d.diagnosis_comment, '') as `Diagnosis Comment`,
 coalesce(d.disease_phase, '') as `Disease Phase`,
 coalesce(d.anatomic_site, '') as `Anatomic Site`,
-coalesce(d.age_at_diagnosis, '') as `Age at diagnosis (days)`,
+case d.age_at_diagnosis when -999 then 'Not Reported' else coalesce(d.age_at_diagnosis, '') end as `Age at diagnosis (days)`,
 coalesce(fo.vital_status, '') as `Vital Status`
-Order by p.participant_id  </t>
+Order by p.participant_id limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+where st.phs_accession in ["phs003111"]
+with st, count(p) as num_p
+MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
+ORDER BY num_cancers desc
+with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
+MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
+with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
+ORDER BY num_sites desc
+with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
+MATCH (st)&lt;-[*..5]-(fl)
+WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:radiology_file OR fl:methylation_array_file OR fl:single_cell_sequencing_file OR fl:cytogenomic_file)
+with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
+ORDER BY num_ft desc
+with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
+OPTIONAL MATCH (st)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm1:sample)
+WHERE (pcp:participant or pcp:cell_line or pcp:pdx)
+WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm1.sample_id) as num_samples_1
+OPTIONAL MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
+WHERE (cp:cell_line or cp:pdx)
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1, count(distinct sm2.sample_id) as num_samples_2
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1 + num_samples_2 as num_samples
+MATCH (st)&lt;-[*..5]-(file)
+WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+WHERE stp.personnel_type = 'PI'
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
+order by st.study_id
+RETURN DISTINCT
+  st.study_short_title as `Study Short Title`,
+st.study_id as `Study ID`,
+  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "Read More"  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
+  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "Read More"  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
+  num_p as `Number of Participants`,
+  num_samples as `Number of Samples`,
+  num_files as `Number of Files`,
+  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "Read More"  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
+  apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
+  apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
+  apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +466,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,9 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -723,17 +822,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="92.42578125" customWidth="1"/>
     <col min="3" max="3" width="86.140625" customWidth="1"/>
     <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,88 +852,88 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="300" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -851,7 +950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ccdi - small updates to the input files based on xl macro
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FD3AD9-768E-4974-A2FB-4E93F0DB4293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDF5F93-ED72-4D97-9060-E73F681C5554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -94,6 +94,97 @@
         count(distinct p.id)as Participants,
           count(distinct sm.id) as Samples,
         count(distinct file.id) as Files</t>
+  </si>
+  <si>
+    <t>CALL {
+  MATCH (st:study)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm:sample)
+  WHERE (pcp:participant or pcp:cell_line or pcp:pdx) and st.phs_accession IN ['phs003111']
+  return st, case labels(pcp)[0] when "participant" then pcp.participant_id else "" end as participant_id, sm
+  union all
+  MATCH (st:study)&lt;-[:of_participant]-(p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
+  WHERE (cp:cell_line or cp:pdx) and st.phs_accession IN ['phs003111']
+  with st, p.participant_id as participant_id, [sm1,sm2] as sampleArr
+  unwind sampleArr as sm
+  return st, participant_id, sm
+}
+RETURN DISTINCT
+          sm.sample_id as `Sample ID`,
+          participant_id as `Participant ID`,
+          st.study_id as `Study ID`,
+          sm.anatomic_site as `Anatomic Site`,
+          case sm.participant_age_at_collection when -999 then 'Not Reported' else coalesce(sm.participant_age_at_collection, '') end as `Age at Sample Collection`,
+          coalesce(sm.diagnosis_classification, '') as `Diagnosis`,
+          coalesce(sm.diagnosis_classification_system, '') as `Diagnosis Classification System`,
+          coalesce(sm.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
+          coalesce(sm.diagnosis_basis, '') as `Diagnosis Basis`,
+          coalesce(sm.diagnosis_comment, '') as `Diagnosis Comment`,
+          sm.sample_tumor_status as `Sample Tumor Status`,
+          sm.tumor_classification as `Sample Tumor Classification`
+Order by sm.sample_id Limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+where st.phs_accession in ["phs003111"]
+with st, count(p) as num_p
+MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
+ORDER BY num_cancers desc
+with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
+MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
+with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
+ORDER BY num_sites desc
+with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
+MATCH (st)&lt;-[*..5]-(fl)
+WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:radiology_file OR fl:methylation_array_file OR fl:single_cell_sequencing_file OR fl:cytogenomic_file)
+with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
+ORDER BY num_ft desc
+with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
+OPTIONAL MATCH (st)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm1:sample)
+WHERE (pcp:participant or pcp:cell_line or pcp:pdx)
+WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm1.sample_id) as num_samples_1
+OPTIONAL MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
+WHERE (cp:cell_line or cp:pdx)
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1, count(distinct sm2.sample_id) as num_samples_2
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1 + num_samples_2 as num_samples
+MATCH (st)&lt;-[*..5]-(file)
+WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+WHERE stp.personnel_type = 'PI'
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
+order by st.study_id
+RETURN DISTINCT
+  st.study_short_title as `Study Short Title`,
+st.study_id as `Study ID`,
+  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "Read More"  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
+  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "Read More"  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
+  num_p as `Number of Participants`,
+  num_samples as `Number of Samples`,
+  num_files as `Number of Files`,
+  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "Read More"  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
+  apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
+  apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
+  apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
+  </si>
+  <si>
+    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
+where s.phs_accession = "phs003111"
+OPTIONAL MATCH(fo:follow_up)--&gt;(p)
+with distinct d, p, s, fo
+return
+coalesce(p.participant_id, '') as `Participant ID`,
+coalesce(s.phs_accession, '') as `Study ID`,
+coalesce(d.diagnosis_classification, '') as `Diagnosis`,
+coalesce(d.diagnosis_classification_system, '') as `Diagnosis Classification System`,
+coalesce(d.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
+coalesce(d.diagnosis_basis, '') as `Diagnosis Basis`,
+coalesce(d.diagnosis_comment, '') as `Diagnosis Comment`,
+coalesce(d.disease_phase, '') as `Disease Phase`,
+coalesce(d.anatomic_site, '') as `Anatomic Site`,
+case d.age_at_diagnosis when -999 then 'Not Reported' else coalesce(d.age_at_diagnosis, '') end as `Age at Diagnosis (days)`,
+coalesce(fo.vital_status, '') as `Vital Status`
+Order by p.participant_id limit 100</t>
   </si>
   <si>
     <t>CALL {
@@ -350,99 +441,8 @@
 participant_id As `Participant ID`,
 sample_id As `Sample ID`,
 guid As `GUID`,
-md5sum As `MD5Sum`
+md5sum As `MD5sum`
 ORDER BY file_name LIMIT 100</t>
-  </si>
-  <si>
-    <t>CALL {
-  MATCH (st:study)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm:sample)
-  WHERE (pcp:participant or pcp:cell_line or pcp:pdx) and st.phs_accession IN ['phs003111']
-  return st, case labels(pcp)[0] when "participant" then pcp.participant_id else "" end as participant_id, sm
-  union all
-  MATCH (st:study)&lt;-[:of_participant]-(p:participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
-  WHERE (cp:cell_line or cp:pdx) and st.phs_accession IN ['phs003111']
-  with st, p.participant_id as participant_id, [sm1,sm2] as sampleArr
-  unwind sampleArr as sm
-  return st, participant_id, sm
-}
-RETURN DISTINCT
-          sm.sample_id as `Sample ID`,
-          participant_id as `Participant ID`,
-          st.study_id as `Study ID`,
-          sm.anatomic_site as `Anatomic Site`,
-          case sm.participant_age_at_collection when -999 then 'Not Reported' else coalesce(sm.participant_age_at_collection, '') end as `Age at Sample Collection`,
-          coalesce(sm.diagnosis_classification, '') as `Diagnosis`,
-          coalesce(sm.diagnosis_classification_system, '') as `Diagnosis Classification System`,
-          coalesce(sm.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
-          coalesce(sm.diagnosis_basis, '') as `Diagnosis Basis`,
-          coalesce(sm.diagnosis_comment, '') as `Diagnosis Comment`,
-          sm.sample_tumor_status as `Sample Tumor Status`,
-          sm.tumor_classification as `Sample Tumor Classification`
-Order by sm.sample_id Limit 100</t>
-  </si>
-  <si>
-    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
-where s.phs_accession = "phs003111"
-OPTIONAL MATCH(fo:follow_up)--&gt;(p)
-with distinct d, p, s, fo
-return
-coalesce(p.participant_id, '') as `Participant ID`,
-coalesce(s.phs_accession, '') as `Study ID`,
-coalesce(d.diagnosis_classification, '') as `Diagnosis`,
-coalesce(d.diagnosis_classification_system, '') as `Diagnosis Classification System`,
-coalesce(d.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
-coalesce(d.diagnosis_basis, '') as `Diagnosis Basis`,
-coalesce(d.diagnosis_comment, '') as `Diagnosis Comment`,
-coalesce(d.disease_phase, '') as `Disease Phase`,
-coalesce(d.anatomic_site, '') as `Anatomic Site`,
-case d.age_at_diagnosis when -999 then 'Not Reported' else coalesce(d.age_at_diagnosis, '') end as `Age at diagnosis (days)`,
-coalesce(fo.vital_status, '') as `Vital Status`
-Order by p.participant_id limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-where st.phs_accession in ["phs003111"]
-with st, count(p) as num_p
-MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
-with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
-ORDER BY num_cancers desc
-with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
-MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
-with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
-ORDER BY num_sites desc
-with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
-MATCH (st)&lt;-[*..5]-(fl)
-WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:radiology_file OR fl:methylation_array_file OR fl:single_cell_sequencing_file OR fl:cytogenomic_file)
-with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
-ORDER BY num_ft desc
-with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
-OPTIONAL MATCH (st)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm1:sample)
-WHERE (pcp:participant or pcp:cell_line or pcp:pdx)
-WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm1.sample_id) as num_samples_1
-OPTIONAL MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
-WHERE (cp:cell_line or cp:pdx)
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1, count(distinct sm2.sample_id) as num_samples_2
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1 + num_samples_2 as num_samples
-MATCH (st)&lt;-[*..5]-(file)
-WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-WHERE stp.personnel_type = 'PI'
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
-order by st.study_id
-RETURN DISTINCT
-  st.study_short_title as `Study Short Title`,
-st.study_id as `Study ID`,
-  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "Read More"  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
-  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "Read More"  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
-  num_p as `Number of Participants`,
-  num_samples as `Number of Samples`,
-  num_files as `Number of Files`,
-  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "Read More"  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
-  apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
-  apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
-  apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
 </sst>
 </file>
@@ -820,10 +820,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +892,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -908,7 +909,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
@@ -925,7 +926,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
@@ -946,6 +947,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D94671-34CB-46BD-8964-4DC9A3E8B07A}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
CDS automation curation - only phs
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_Filter_PHS-Accession-phs003111.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDF5F93-ED72-4D97-9060-E73F681C5554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF4CF8B-ED7F-4E85-A41F-D0011A2F1247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -81,19 +81,6 @@
 coalesce(p.ethnicity, '') AS `Ethnicity` ,
 coalesce(p.alternate_participant_id, '') AS `Alternate ID`
 Order by p.participant_id Limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-WHERE  st.phs_accession IN ['phs003111']
-        OPTIONAL MATCH (st)&lt;-[*..5]-(file)
-        WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:rathology OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-        WITH file, p, st, sm
-        return
-        count(distinct st.id) as Studies,
-        count(distinct p.id)as Participants,
-          count(distinct sm.id) as Samples,
-        count(distinct file.id) as Files</t>
   </si>
   <si>
     <t>CALL {
@@ -123,8 +110,27 @@
 Order by sm.sample_id Limit 100</t>
   </si>
   <si>
+    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
+where s.phs_accession = "phs003111"
+OPTIONAL MATCH(fo:follow_up)--&gt;(p)
+with distinct d, p, s, fo
+return
+coalesce(p.participant_id, '') as `Participant ID`,
+coalesce(s.phs_accession, '') as `Study ID`,
+coalesce(d.diagnosis_classification, '') as `Diagnosis`,
+coalesce(d.diagnosis_classification_system, '') as `Diagnosis Classification System`,
+coalesce(d.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
+coalesce(d.diagnosis_basis, '') as `Diagnosis Basis`,
+coalesce(d.diagnosis_comment, '') as `Diagnosis Comment`,
+coalesce(d.disease_phase, '') as `Disease Phase`,
+coalesce(d.anatomic_site, '') as `Anatomic Site`,
+case d.age_at_diagnosis when -999 then 'Not Reported' else coalesce(d.age_at_diagnosis, '') end as `Age at Diagnosis (days)`,
+coalesce(fo.vital_status, '') as `Vital Status`
+Order by p.participant_id limit 100</t>
+  </si>
+  <si>
     <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-where st.phs_accession in ["phs003111"]
+where st.phs_accession in ["phs002430"]
 with st, count(p) as num_p
 MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
 with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
@@ -157,34 +163,28 @@
 RETURN DISTINCT
   st.study_short_title as `Study Short Title`,
 st.study_id as `Study ID`,
-  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "") + "Read More"  else apoc.text.join(cancers, "") END as `Diagnosis (Top 5)`,
-  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "") + "Read More"  else apoc.text.join(sites, "") END as `Diagnosis Anatomic Site (Top 5)`,
+  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(cancers, "\n") END as `Diagnosis (Top 5)`,
+  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(sites, "\n") END as `Diagnosis Anatomic Site (Top 5)`,
   num_p as `Number of Participants`,
   num_samples as `Number of Samples`,
   num_files as `Number of Files`,
-  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "Read More"  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
+  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(file_types, "\n") END as `File Type (Top 5)`,
   apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
   apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
   apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
   <si>
-    <t>Match (s:study)&lt;--(p:participant)&lt;--(d:diagnosis)
-where s.phs_accession = "phs003111"
-OPTIONAL MATCH(fo:follow_up)--&gt;(p)
-with distinct d, p, s, fo
-return
-coalesce(p.participant_id, '') as `Participant ID`,
-coalesce(s.phs_accession, '') as `Study ID`,
-coalesce(d.diagnosis_classification, '') as `Diagnosis`,
-coalesce(d.diagnosis_classification_system, '') as `Diagnosis Classification System`,
-coalesce(d.diagnosis_verification_status, '') as `Diagnosis Verification Status`,
-coalesce(d.diagnosis_basis, '') as `Diagnosis Basis`,
-coalesce(d.diagnosis_comment, '') as `Diagnosis Comment`,
-coalesce(d.disease_phase, '') as `Disease Phase`,
-coalesce(d.anatomic_site, '') as `Anatomic Site`,
-case d.age_at_diagnosis when -999 then 'Not Reported' else coalesce(d.age_at_diagnosis, '') end as `Age at Diagnosis (days)`,
-coalesce(fo.vital_status, '') as `Vital Status`
-Order by p.participant_id limit 100</t>
+    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+WHERE  st.phs_accession IN ['phs003111']
+        OPTIONAL MATCH (st)&lt;-[*..5]-(file)
+        WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
+        WITH file, p, st, sm
+        return
+        count(distinct st.id) as Studies,
+        count(distinct p.id)as Participants,
+          count(distinct sm.id) as Samples,
+        count(distinct file.id) as Files</t>
   </si>
   <si>
     <t>CALL {
@@ -441,7 +441,7 @@
 participant_id As `Participant ID`,
 sample_id As `Sample ID`,
 guid As `GUID`,
-md5sum As `MD5sum`
+md5sum As `MD5Sum`
 ORDER BY file_name LIMIT 100</t>
   </si>
 </sst>
@@ -823,8 +823,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -875,10 +875,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -895,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -909,10 +909,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -929,7 +929,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>

</xml_diff>